<commit_message>
fix: allow tokenizer to consume all characters other than flag markers as part of the text
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="119">
   <si>
     <t>Word</t>
   </si>
@@ -32,12 +32,24 @@
     <t>Created at</t>
   </si>
   <si>
+    <t>condescending</t>
+  </si>
+  <si>
+    <t>having or showing an attitude of patronizing superiority</t>
+  </si>
+  <si>
+    <t>patronizing</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2021-10-28 00:12:08.521439</t>
+  </si>
+  <si>
     <t>debacle</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>fiasco</t>
   </si>
   <si>
@@ -80,6 +92,9 @@
     <t>onerous</t>
   </si>
   <si>
+    <t>involving a great deal of effort, trouble or difficulty</t>
+  </si>
+  <si>
     <t>burdensome</t>
   </si>
   <si>
@@ -149,18 +164,6 @@
     <t>2021-10-28 00:31:41.851617</t>
   </si>
   <si>
-    <t>condescending</t>
-  </si>
-  <si>
-    <t>having or showing an attitude of patronizing superiority</t>
-  </si>
-  <si>
-    <t>patronizing</t>
-  </si>
-  <si>
-    <t>2021-10-28 00:12:08.521439</t>
-  </si>
-  <si>
     <t>unhinged</t>
   </si>
   <si>
@@ -171,6 +174,201 @@
   </si>
   <si>
     <t>2021-11-05 22:58:27.652222</t>
+  </si>
+  <si>
+    <t>perpetrate</t>
+  </si>
+  <si>
+    <t>carry out or commit (a harmful, illegal, or immoral action)</t>
+  </si>
+  <si>
+    <t>commit</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:09:26.006923</t>
+  </si>
+  <si>
+    <t>incentive</t>
+  </si>
+  <si>
+    <t>a thing that motivates or encourages someone to do something</t>
+  </si>
+  <si>
+    <t>inducement</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:10:54.925723</t>
+  </si>
+  <si>
+    <t>ramification</t>
+  </si>
+  <si>
+    <t>consequence</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:12:12.541448</t>
+  </si>
+  <si>
+    <t>apoptosis</t>
+  </si>
+  <si>
+    <t>the death of cells which occurs as a normal and controlled part of an organism's growth or development</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:13:34.20914</t>
+  </si>
+  <si>
+    <t>recuperate</t>
+  </si>
+  <si>
+    <t>recover from illness or exertion</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:14:29.445691</t>
+  </si>
+  <si>
+    <t>felony</t>
+  </si>
+  <si>
+    <t>a violent and terrible crime</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:17:05.669846</t>
+  </si>
+  <si>
+    <t>peddle</t>
+  </si>
+  <si>
+    <t>sell;advocate</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:18:45.861368</t>
+  </si>
+  <si>
+    <t>fallacy</t>
+  </si>
+  <si>
+    <t>a mistaken belief, especially one based on unsound arguments</t>
+  </si>
+  <si>
+    <t>misconception</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:19:33.647009</t>
+  </si>
+  <si>
+    <t>stupor</t>
+  </si>
+  <si>
+    <t>a state of near-unconsciousness or insensibility</t>
+  </si>
+  <si>
+    <t>daze</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:20:57.383103</t>
+  </si>
+  <si>
+    <t>foyer</t>
+  </si>
+  <si>
+    <t>entrance hall</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:21:33.130184</t>
+  </si>
+  <si>
+    <t>pundit</t>
+  </si>
+  <si>
+    <t>expert</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:23:13.008626</t>
+  </si>
+  <si>
+    <t>lambast</t>
+  </si>
+  <si>
+    <t>criticize harshly</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:26:18.659339</t>
+  </si>
+  <si>
+    <t>soar</t>
+  </si>
+  <si>
+    <t>increasing rapidly above the usual level</t>
+  </si>
+  <si>
+    <t>fly up</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:27:02.200839</t>
+  </si>
+  <si>
+    <t>intact</t>
+  </si>
+  <si>
+    <t>not damaged or impaired in any way; complete</t>
+  </si>
+  <si>
+    <t>whole</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:27:50.644715</t>
+  </si>
+  <si>
+    <t>shoddy</t>
+  </si>
+  <si>
+    <t>careless;poor-quality</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:28:42.360492</t>
+  </si>
+  <si>
+    <t>tattered</t>
+  </si>
+  <si>
+    <t>old and torn; in poor condition</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:30:10.930195</t>
+  </si>
+  <si>
+    <t>inherent</t>
+  </si>
+  <si>
+    <t>existing in something as a permanent, essential, or characteristic attribute</t>
+  </si>
+  <si>
+    <t>intrinsic</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:31:22.01212</t>
+  </si>
+  <si>
+    <t>decry</t>
+  </si>
+  <si>
+    <t>denounce</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:32:11.165969</t>
+  </si>
+  <si>
+    <t>frenetic</t>
+  </si>
+  <si>
+    <t>fast and energetic in a rather wild and uncontrolled way</t>
+  </si>
+  <si>
+    <t>frantic</t>
+  </si>
+  <si>
+    <t>2021-11-05 23:32:57.751058</t>
   </si>
 </sst>
 </file>
@@ -215,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -252,293 +450,673 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="n">
         <v>0.0</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E3" t="n">
         <v>0.0</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E4" t="n">
         <v>0.0</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
         <v>0.0</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E6" t="n">
         <v>0.0</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E7" t="n">
         <v>0.0</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E8" t="n">
         <v>0.0</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E9" t="n">
         <v>0.0</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E10" t="n">
         <v>0.0</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E11" t="n">
         <v>0.0</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E12" t="n">
         <v>0.0</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E13" t="n">
         <v>0.0</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E14" t="n">
         <v>0.0</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E15" t="n">
         <v>0.0</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E16" t="n">
         <v>0.0</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: simplify sql queries when fetching words for the vocabulary training session
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="295">
   <si>
     <t>Word</t>
   </si>
@@ -771,6 +771,60 @@
     <t>2021-11-14 00:25:37.291554</t>
   </si>
   <si>
+    <t>erratic</t>
+  </si>
+  <si>
+    <t>unpredictable</t>
+  </si>
+  <si>
+    <t>2021-11-14 16:37:51.305571</t>
+  </si>
+  <si>
+    <t>entail</t>
+  </si>
+  <si>
+    <t>involve (smth) as a necessary or inevitable part or consequence</t>
+  </si>
+  <si>
+    <t>necessitate</t>
+  </si>
+  <si>
+    <t>2021-11-14 16:39:12.99207</t>
+  </si>
+  <si>
+    <t>disengage</t>
+  </si>
+  <si>
+    <t>remove;withdraw</t>
+  </si>
+  <si>
+    <t>2021-11-14 16:45:31.492612</t>
+  </si>
+  <si>
+    <t>recuperation</t>
+  </si>
+  <si>
+    <t>recovery from illness or exertion</t>
+  </si>
+  <si>
+    <t>recovery</t>
+  </si>
+  <si>
+    <t>2021-11-14 16:46:27.758408</t>
+  </si>
+  <si>
+    <t>nurture</t>
+  </si>
+  <si>
+    <t>care for and protect (someone or smth) while they are growing</t>
+  </si>
+  <si>
+    <t>cultivate</t>
+  </si>
+  <si>
+    <t>2021-11-14 16:48:04.864399</t>
+  </si>
+  <si>
     <t>content</t>
   </si>
   <si>
@@ -829,6 +883,21 @@
   </si>
   <si>
     <t>Saying what you mean and meaning what you say</t>
+  </si>
+  <si>
+    <t>Each night, when I go to sleep, I die. And the next morning, when I wake up, I am reborn</t>
+  </si>
+  <si>
+    <t>If the answer isn't a definite yes then it should be a no</t>
+  </si>
+  <si>
+    <t>If it isn't a clear yes, then it's a clear no</t>
+  </si>
+  <si>
+    <t>To follow, without halt, one aim: there is the secret to success</t>
+  </si>
+  <si>
+    <t>Half of the troubles of this life can be traced to saying yes too quickly and not saying no soon enough</t>
   </si>
 </sst>
 </file>
@@ -873,7 +942,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2379,6 +2448,106 @@
         <v>251</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>252</v>
+      </c>
+      <c r="B76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" t="s">
+        <v>253</v>
+      </c>
+      <c r="D76" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F76" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>255</v>
+      </c>
+      <c r="B77" t="s">
+        <v>256</v>
+      </c>
+      <c r="C77" t="s">
+        <v>257</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F77" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>259</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" t="s">
+        <v>260</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F78" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>262</v>
+      </c>
+      <c r="B79" t="s">
+        <v>263</v>
+      </c>
+      <c r="C79" t="s">
+        <v>264</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F79" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>266</v>
+      </c>
+      <c r="B80" t="s">
+        <v>267</v>
+      </c>
+      <c r="C80" t="s">
+        <v>268</v>
+      </c>
+      <c r="D80" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>269</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2386,7 +2555,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2394,102 +2563,127 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>271</v>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add command to attach tags to notes and vocabulary entries
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="345">
   <si>
     <t>Word</t>
   </si>
@@ -823,6 +823,156 @@
   </si>
   <si>
     <t>2021-11-14 16:48:04.864399</t>
+  </si>
+  <si>
+    <t>fatigue</t>
+  </si>
+  <si>
+    <t>tiredness</t>
+  </si>
+  <si>
+    <t>2021-11-14 20:15:38.955425</t>
+  </si>
+  <si>
+    <t>cumulatively</t>
+  </si>
+  <si>
+    <t>in a way that increases in quantity, degree, or force by successive addition</t>
+  </si>
+  <si>
+    <t>2021-11-14 20:16:29.606448</t>
+  </si>
+  <si>
+    <t>ample</t>
+  </si>
+  <si>
+    <t>enough;plentiful</t>
+  </si>
+  <si>
+    <t>2021-11-14 20:17:00.34091</t>
+  </si>
+  <si>
+    <t>pernicious</t>
+  </si>
+  <si>
+    <t>harmful</t>
+  </si>
+  <si>
+    <t>2021-11-14 20:17:55.875123</t>
+  </si>
+  <si>
+    <t>liken</t>
+  </si>
+  <si>
+    <t>point out the resemblance of someone or smth to</t>
+  </si>
+  <si>
+    <t>compare</t>
+  </si>
+  <si>
+    <t>2021-11-14 20:18:50.405149</t>
+  </si>
+  <si>
+    <t>machismo</t>
+  </si>
+  <si>
+    <t>aggresive masculinity</t>
+  </si>
+  <si>
+    <t>2021-11-15 14:49:54.205507</t>
+  </si>
+  <si>
+    <t>stigma</t>
+  </si>
+  <si>
+    <t>a mark of disgrace associated with a particular circumstance, quality, or person</t>
+  </si>
+  <si>
+    <t>shame</t>
+  </si>
+  <si>
+    <t>2021-11-15 14:50:45.332093</t>
+  </si>
+  <si>
+    <t>commodity</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>2021-11-15 14:51:17.949615</t>
+  </si>
+  <si>
+    <t>deride</t>
+  </si>
+  <si>
+    <t>express contempt for</t>
+  </si>
+  <si>
+    <t>ridicule</t>
+  </si>
+  <si>
+    <t>2021-11-15 14:51:56.068144</t>
+  </si>
+  <si>
+    <t>wimpish</t>
+  </si>
+  <si>
+    <t>weak and cowardly or unadventurous</t>
+  </si>
+  <si>
+    <t>2021-11-15 14:52:35.494874</t>
+  </si>
+  <si>
+    <t>tout</t>
+  </si>
+  <si>
+    <t>attempt to sell smth, typically by a direct or persistent approach</t>
+  </si>
+  <si>
+    <t>peddle;solicit</t>
+  </si>
+  <si>
+    <t>2021-11-15 14:53:45.152971</t>
+  </si>
+  <si>
+    <t>discerning</t>
+  </si>
+  <si>
+    <t>having or showing good judgement</t>
+  </si>
+  <si>
+    <t>2021-11-15 14:54:30.922667</t>
+  </si>
+  <si>
+    <t>mediocre</t>
+  </si>
+  <si>
+    <t>of only average quality; not very good</t>
+  </si>
+  <si>
+    <t>ordinary</t>
+  </si>
+  <si>
+    <t>2021-11-15 14:55:50.807842</t>
+  </si>
+  <si>
+    <t>utter</t>
+  </si>
+  <si>
+    <t>absolute;complete</t>
+  </si>
+  <si>
+    <t>2021-11-15 14:56:38.984503</t>
+  </si>
+  <si>
+    <t>conviction</t>
+  </si>
+  <si>
+    <t>belief</t>
+  </si>
+  <si>
+    <t>2021-11-15 14:57:11.455154</t>
   </si>
   <si>
     <t>content</t>
@@ -942,7 +1092,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2546,6 +2696,306 @@
       </c>
       <c r="F80" t="s">
         <v>269</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>270</v>
+      </c>
+      <c r="B81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" t="s">
+        <v>271</v>
+      </c>
+      <c r="D81" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F81" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>273</v>
+      </c>
+      <c r="B82" t="s">
+        <v>274</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F82" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>276</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" t="s">
+        <v>277</v>
+      </c>
+      <c r="D83" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F83" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>279</v>
+      </c>
+      <c r="B84" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84" t="s">
+        <v>280</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F84" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>282</v>
+      </c>
+      <c r="B85" t="s">
+        <v>283</v>
+      </c>
+      <c r="C85" t="s">
+        <v>284</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F85" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>286</v>
+      </c>
+      <c r="B86" t="s">
+        <v>287</v>
+      </c>
+      <c r="C86" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F86" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>289</v>
+      </c>
+      <c r="B87" t="s">
+        <v>290</v>
+      </c>
+      <c r="C87" t="s">
+        <v>291</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F87" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>293</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" t="s">
+        <v>294</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F88" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>296</v>
+      </c>
+      <c r="B89" t="s">
+        <v>297</v>
+      </c>
+      <c r="C89" t="s">
+        <v>298</v>
+      </c>
+      <c r="D89" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F89" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>300</v>
+      </c>
+      <c r="B90" t="s">
+        <v>301</v>
+      </c>
+      <c r="C90" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F90" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>303</v>
+      </c>
+      <c r="B91" t="s">
+        <v>304</v>
+      </c>
+      <c r="C91" t="s">
+        <v>305</v>
+      </c>
+      <c r="D91" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F91" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>307</v>
+      </c>
+      <c r="B92" t="s">
+        <v>308</v>
+      </c>
+      <c r="C92" t="s">
+        <v>9</v>
+      </c>
+      <c r="D92" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F92" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>310</v>
+      </c>
+      <c r="B93" t="s">
+        <v>311</v>
+      </c>
+      <c r="C93" t="s">
+        <v>312</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F93" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>314</v>
+      </c>
+      <c r="B94" t="s">
+        <v>9</v>
+      </c>
+      <c r="C94" t="s">
+        <v>315</v>
+      </c>
+      <c r="D94" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F94" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>317</v>
+      </c>
+      <c r="B95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" t="s">
+        <v>318</v>
+      </c>
+      <c r="D95" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F95" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -2563,127 +3013,127 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>270</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>272</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>274</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>275</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>276</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>277</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>278</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>279</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>280</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>281</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>282</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>283</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>284</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>285</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>286</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>287</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>288</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>289</v>
+        <v>339</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>290</v>
+        <v>340</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>292</v>
+        <v>342</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>293</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>294</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: load tags when displaying notes and vocabulary entries
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="377">
   <si>
     <t>Word</t>
   </si>
@@ -975,6 +975,99 @@
     <t>2021-11-15 14:57:11.455154</t>
   </si>
   <si>
+    <t>unenviable</t>
+  </si>
+  <si>
+    <t>unpleasant;difficult;undesirable</t>
+  </si>
+  <si>
+    <t>2021-11-16 12:53:53.320239</t>
+  </si>
+  <si>
+    <t>vigilant</t>
+  </si>
+  <si>
+    <t>watchful</t>
+  </si>
+  <si>
+    <t>2021-11-16 12:54:22.449368</t>
+  </si>
+  <si>
+    <t>amplify</t>
+  </si>
+  <si>
+    <t>expand;louden</t>
+  </si>
+  <si>
+    <t>2021-11-16 12:54:56.705918</t>
+  </si>
+  <si>
+    <t>notorious</t>
+  </si>
+  <si>
+    <t>well known, typically for some bad quality or deed</t>
+  </si>
+  <si>
+    <t>infamous</t>
+  </si>
+  <si>
+    <t>2021-11-16 12:55:49.850794</t>
+  </si>
+  <si>
+    <t>epitomize</t>
+  </si>
+  <si>
+    <t>summarize;embody</t>
+  </si>
+  <si>
+    <t>2021-11-16 12:56:33.27447</t>
+  </si>
+  <si>
+    <t>rigorous</t>
+  </si>
+  <si>
+    <t>extremely thorough and careful</t>
+  </si>
+  <si>
+    <t>strict;meticulous</t>
+  </si>
+  <si>
+    <t>2021-11-16 12:57:47.829373</t>
+  </si>
+  <si>
+    <t>weed out</t>
+  </si>
+  <si>
+    <t>isolate</t>
+  </si>
+  <si>
+    <t>2021-11-16 12:59:23.223598</t>
+  </si>
+  <si>
+    <t>debrief</t>
+  </si>
+  <si>
+    <t>question (someone, typically a soldier or spy) about a completed mission</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>2021-11-16 13:00:53.826091</t>
+  </si>
+  <si>
+    <t>infraction</t>
+  </si>
+  <si>
+    <t>a violation of a law or agreement</t>
+  </si>
+  <si>
+    <t>infringement</t>
+  </si>
+  <si>
+    <t>2021-11-16 13:01:47.533568</t>
+  </si>
+  <si>
     <t>content</t>
   </si>
   <si>
@@ -1048,6 +1141,9 @@
   </si>
   <si>
     <t>Half of the troubles of this life can be traced to saying yes too quickly and not saying no soon enough</t>
+  </si>
+  <si>
+    <t>Less but better</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1188,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2998,6 +3094,186 @@
         <v>319</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>320</v>
+      </c>
+      <c r="B96" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" t="s">
+        <v>321</v>
+      </c>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F96" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>323</v>
+      </c>
+      <c r="B97" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" t="s">
+        <v>324</v>
+      </c>
+      <c r="D97" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F97" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>326</v>
+      </c>
+      <c r="B98" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98" t="s">
+        <v>327</v>
+      </c>
+      <c r="D98" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F98" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>329</v>
+      </c>
+      <c r="B99" t="s">
+        <v>330</v>
+      </c>
+      <c r="C99" t="s">
+        <v>331</v>
+      </c>
+      <c r="D99" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F99" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>333</v>
+      </c>
+      <c r="B100" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100" t="s">
+        <v>334</v>
+      </c>
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F100" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>336</v>
+      </c>
+      <c r="B101" t="s">
+        <v>337</v>
+      </c>
+      <c r="C101" t="s">
+        <v>338</v>
+      </c>
+      <c r="D101" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F101" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>340</v>
+      </c>
+      <c r="B102" t="s">
+        <v>9</v>
+      </c>
+      <c r="C102" t="s">
+        <v>341</v>
+      </c>
+      <c r="D102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F102" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>343</v>
+      </c>
+      <c r="B103" t="s">
+        <v>344</v>
+      </c>
+      <c r="C103" t="s">
+        <v>345</v>
+      </c>
+      <c r="D103" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F103" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>347</v>
+      </c>
+      <c r="B104" t="s">
+        <v>348</v>
+      </c>
+      <c r="C104" t="s">
+        <v>349</v>
+      </c>
+      <c r="D104" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F104" t="s">
+        <v>350</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -3005,7 +3281,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3013,127 +3289,132 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>320</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>321</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>322</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>323</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>324</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>325</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>326</v>
+        <v>357</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>327</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>328</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>329</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>330</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>331</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>332</v>
+        <v>363</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>333</v>
+        <v>364</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>334</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>335</v>
+        <v>366</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>336</v>
+        <v>367</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>337</v>
+        <v>368</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>338</v>
+        <v>369</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>339</v>
+        <v>370</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>340</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>341</v>
+        <v>372</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>342</v>
+        <v>373</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>343</v>
+        <v>374</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>344</v>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: allow creating notes and vocabulary entries with tags
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ENGLISH" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="446">
   <si>
     <t xml:space="preserve">Word</t>
   </si>
@@ -698,7 +698,7 @@
     <t xml:space="preserve">2021-11-13 15:27:25.556179</t>
   </si>
   <si>
-    <t xml:space="preserve">disentabgle</t>
+    <t xml:space="preserve">disentangle</t>
   </si>
   <si>
     <t xml:space="preserve">free from something that they are entangled with</t>
@@ -1181,6 +1181,102 @@
     <t xml:space="preserve">2021-11-17 13:05:11.821048</t>
   </si>
   <si>
+    <t xml:space="preserve">resentment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bitterness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-18 13:38:55.766952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coalesce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com together to form one mass or whole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-18 13:39:52.321676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">easily frightened</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-18 13:40:17.759858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reverberation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prolongation of a sound; a continuing effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resonance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-18 13:41:26.98325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imprisonment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incarceration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-18 13:42:08.650617</t>
+  </si>
+  <si>
+    <t xml:space="preserve">convention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agreement;custom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-18 13:44:21.614304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crestfallen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disappointed;downhearted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-18 13:45:08.281708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">innate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natural;inborn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-18 13:46:56.18276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">muddle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confuse;bewilder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-18 13:47:26.716003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resolutely</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in an admirably purposeful, determined, and unwavering manner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-18 13:48:20.311353</t>
+  </si>
+  <si>
     <t xml:space="preserve">content</t>
   </si>
   <si>
@@ -1260,6 +1356,9 @@
   </si>
   <si>
     <t xml:space="preserve">Less but better</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The main thing is to keep the main thing the main thing</t>
   </si>
 </sst>
 </file>
@@ -1355,10 +1454,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3089,6 +3188,152 @@
       </c>
       <c r="F114" s="0" t="s">
         <v>385</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="E115" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F115" s="0" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="E116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F116" s="0" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="E117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" s="0" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="E118" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F118" s="0" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="E119" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F119" s="0" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="E120" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F120" s="0" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="E121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" s="0" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="E122" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F122" s="0" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="E123" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F123" s="0" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="E124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F124" s="0" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -3107,17 +3352,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>386</v>
+        <v>418</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>6</v>
@@ -3125,133 +3370,141 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>387</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>388</v>
+        <v>420</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>389</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>390</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>391</v>
+        <v>423</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>392</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>393</v>
+        <v>425</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>394</v>
+        <v>426</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>395</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>396</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>397</v>
+        <v>429</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>398</v>
+        <v>430</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>399</v>
+        <v>431</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>400</v>
+        <v>432</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>401</v>
+        <v>433</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>402</v>
+        <v>434</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>403</v>
+        <v>435</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>404</v>
+        <v>436</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>405</v>
+        <v>437</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>406</v>
+        <v>438</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>407</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>408</v>
+        <v>440</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>409</v>
+        <v>441</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>410</v>
+        <v>442</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>411</v>
+        <v>443</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>412</v>
+        <v>444</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>411</v>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: simplify the TagDao; access TagDao only from within the TagService
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="520">
   <si>
     <t>Word</t>
   </si>
@@ -705,6 +705,15 @@
     <t>2021-11-13 15:29:33.972408</t>
   </si>
   <si>
+    <t>extricate</t>
+  </si>
+  <si>
+    <t>free from a constraint or difficulty</t>
+  </si>
+  <si>
+    <t>2021-11-20 14:57:27.485397</t>
+  </si>
+  <si>
     <t>slumber</t>
   </si>
   <si>
@@ -1368,6 +1377,96 @@
     <t>2021-11-19 15:04:55.573824</t>
   </si>
   <si>
+    <t>restrained</t>
+  </si>
+  <si>
+    <t>self-controlled</t>
+  </si>
+  <si>
+    <t>2021-11-20 15:03:49.858279</t>
+  </si>
+  <si>
+    <t>condense</t>
+  </si>
+  <si>
+    <t>make denser or more concentrated</t>
+  </si>
+  <si>
+    <t>2021-11-20 15:04:42.212772</t>
+  </si>
+  <si>
+    <t>apt</t>
+  </si>
+  <si>
+    <t>inclined;suitable</t>
+  </si>
+  <si>
+    <t>2021-11-20 15:05:21.928371</t>
+  </si>
+  <si>
+    <t>sentiment</t>
+  </si>
+  <si>
+    <t>a view or opinion that is held or expressed</t>
+  </si>
+  <si>
+    <t>view;feeling</t>
+  </si>
+  <si>
+    <t>2021-11-20 15:06:18.444516</t>
+  </si>
+  <si>
+    <t>fuming</t>
+  </si>
+  <si>
+    <t>feeling, showing or expressing great anger</t>
+  </si>
+  <si>
+    <t>2021-11-20 15:07:39.355342</t>
+  </si>
+  <si>
+    <t>insidiously</t>
+  </si>
+  <si>
+    <t>in a gradual, subtle way, but with harmful effects</t>
+  </si>
+  <si>
+    <t>2021-11-20 15:08:28.761904</t>
+  </si>
+  <si>
+    <t>fret</t>
+  </si>
+  <si>
+    <t>be constantly or visibly anxious</t>
+  </si>
+  <si>
+    <t>worry;trouble</t>
+  </si>
+  <si>
+    <t>2021-11-20 15:10:17.940034</t>
+  </si>
+  <si>
+    <t>unsolicited</t>
+  </si>
+  <si>
+    <t>not asked for; given or done voluntarily</t>
+  </si>
+  <si>
+    <t>uninvited</t>
+  </si>
+  <si>
+    <t>2021-11-20 15:12:00.23661</t>
+  </si>
+  <si>
+    <t>resemble</t>
+  </si>
+  <si>
+    <t>look like</t>
+  </si>
+  <si>
+    <t>2021-11-20 15:12:28.779915</t>
+  </si>
+  <si>
     <t>content</t>
   </si>
   <si>
@@ -1453,6 +1552,27 @@
   </si>
   <si>
     <t>Compoftable with cutting losses</t>
+  </si>
+  <si>
+    <t>Get over the fear of waste</t>
+  </si>
+  <si>
+    <t>Stop making casual commitments</t>
+  </si>
+  <si>
+    <t>Pause before you speak</t>
+  </si>
+  <si>
+    <t>get over the fear of missing out</t>
+  </si>
+  <si>
+    <t>I saw the angel in the marble and carved until I set him free</t>
+  </si>
+  <si>
+    <t>No is a complete sentence</t>
+  </si>
+  <si>
+    <t>If you don't set boundaries - there won't be any</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G134"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -3049,10 +3169,10 @@
         <v>230</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>231</v>
       </c>
       <c r="C68" t="s">
-        <v>231</v>
+        <v>10</v>
       </c>
       <c r="D68" t="s">
         <v>10</v>
@@ -3072,10 +3192,10 @@
         <v>233</v>
       </c>
       <c r="B69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" t="s">
         <v>234</v>
-      </c>
-      <c r="C69" t="s">
-        <v>10</v>
       </c>
       <c r="D69" t="s">
         <v>10</v>
@@ -3095,10 +3215,10 @@
         <v>236</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>237</v>
       </c>
       <c r="C70" t="s">
-        <v>237</v>
+        <v>10</v>
       </c>
       <c r="D70" t="s">
         <v>10</v>
@@ -3190,7 +3310,7 @@
         <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D74" t="s">
         <v>10</v>
@@ -3199,7 +3319,7 @@
         <v>0.0</v>
       </c>
       <c r="F74" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G74" t="s">
         <v>10</v>
@@ -3207,7 +3327,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B75" t="s">
         <v>10</v>
@@ -3256,19 +3376,19 @@
         <v>256</v>
       </c>
       <c r="B77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" t="s">
         <v>257</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F77" t="s">
         <v>258</v>
-      </c>
-      <c r="D77" t="s">
-        <v>10</v>
-      </c>
-      <c r="E77" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F77" t="s">
-        <v>259</v>
       </c>
       <c r="G77" t="s">
         <v>10</v>
@@ -3276,10 +3396,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>259</v>
+      </c>
+      <c r="B78" t="s">
         <v>260</v>
-      </c>
-      <c r="B78" t="s">
-        <v>10</v>
       </c>
       <c r="C78" t="s">
         <v>261</v>
@@ -3302,19 +3422,19 @@
         <v>263</v>
       </c>
       <c r="B79" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" t="s">
         <v>264</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F79" t="s">
         <v>265</v>
-      </c>
-      <c r="D79" t="s">
-        <v>10</v>
-      </c>
-      <c r="E79" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F79" t="s">
-        <v>266</v>
       </c>
       <c r="G79" t="s">
         <v>10</v>
@@ -3322,22 +3442,22 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>266</v>
+      </c>
+      <c r="B80" t="s">
         <v>267</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>268</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F80" t="s">
         <v>269</v>
-      </c>
-      <c r="D80" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F80" t="s">
-        <v>270</v>
       </c>
       <c r="G80" t="s">
         <v>10</v>
@@ -3345,10 +3465,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
+        <v>270</v>
+      </c>
+      <c r="B81" t="s">
         <v>271</v>
-      </c>
-      <c r="B81" t="s">
-        <v>10</v>
       </c>
       <c r="C81" t="s">
         <v>272</v>
@@ -3371,10 +3491,10 @@
         <v>274</v>
       </c>
       <c r="B82" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" t="s">
         <v>275</v>
-      </c>
-      <c r="C82" t="s">
-        <v>10</v>
       </c>
       <c r="D82" t="s">
         <v>10</v>
@@ -3394,10 +3514,10 @@
         <v>277</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>278</v>
       </c>
       <c r="C83" t="s">
-        <v>278</v>
+        <v>10</v>
       </c>
       <c r="D83" t="s">
         <v>10</v>
@@ -3440,19 +3560,19 @@
         <v>283</v>
       </c>
       <c r="B85" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" t="s">
         <v>284</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F85" t="s">
         <v>285</v>
-      </c>
-      <c r="D85" t="s">
-        <v>10</v>
-      </c>
-      <c r="E85" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F85" t="s">
-        <v>286</v>
       </c>
       <c r="G85" t="s">
         <v>10</v>
@@ -3460,13 +3580,13 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
+        <v>286</v>
+      </c>
+      <c r="B86" t="s">
         <v>287</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>288</v>
-      </c>
-      <c r="C86" t="s">
-        <v>10</v>
       </c>
       <c r="D86" t="s">
         <v>10</v>
@@ -3489,16 +3609,16 @@
         <v>291</v>
       </c>
       <c r="C87" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F87" t="s">
         <v>292</v>
-      </c>
-      <c r="D87" t="s">
-        <v>10</v>
-      </c>
-      <c r="E87" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F87" t="s">
-        <v>293</v>
       </c>
       <c r="G87" t="s">
         <v>10</v>
@@ -3506,10 +3626,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
+        <v>293</v>
+      </c>
+      <c r="B88" t="s">
         <v>294</v>
-      </c>
-      <c r="B88" t="s">
-        <v>10</v>
       </c>
       <c r="C88" t="s">
         <v>295</v>
@@ -3532,19 +3652,19 @@
         <v>297</v>
       </c>
       <c r="B89" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" t="s">
         <v>298</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F89" t="s">
         <v>299</v>
-      </c>
-      <c r="D89" t="s">
-        <v>10</v>
-      </c>
-      <c r="E89" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F89" t="s">
-        <v>300</v>
       </c>
       <c r="G89" t="s">
         <v>10</v>
@@ -3552,13 +3672,13 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
+        <v>300</v>
+      </c>
+      <c r="B90" t="s">
         <v>301</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>302</v>
-      </c>
-      <c r="C90" t="s">
-        <v>10</v>
       </c>
       <c r="D90" t="s">
         <v>10</v>
@@ -3581,16 +3701,16 @@
         <v>305</v>
       </c>
       <c r="C91" t="s">
+        <v>10</v>
+      </c>
+      <c r="D91" t="s">
+        <v>10</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F91" t="s">
         <v>306</v>
-      </c>
-      <c r="D91" t="s">
-        <v>10</v>
-      </c>
-      <c r="E91" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F91" t="s">
-        <v>307</v>
       </c>
       <c r="G91" t="s">
         <v>10</v>
@@ -3598,13 +3718,13 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
+        <v>307</v>
+      </c>
+      <c r="B92" t="s">
         <v>308</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>309</v>
-      </c>
-      <c r="C92" t="s">
-        <v>10</v>
       </c>
       <c r="D92" t="s">
         <v>10</v>
@@ -3627,16 +3747,16 @@
         <v>312</v>
       </c>
       <c r="C93" t="s">
+        <v>10</v>
+      </c>
+      <c r="D93" t="s">
+        <v>10</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F93" t="s">
         <v>313</v>
-      </c>
-      <c r="D93" t="s">
-        <v>10</v>
-      </c>
-      <c r="E93" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F93" t="s">
-        <v>314</v>
       </c>
       <c r="G93" t="s">
         <v>10</v>
@@ -3644,10 +3764,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
+        <v>314</v>
+      </c>
+      <c r="B94" t="s">
         <v>315</v>
-      </c>
-      <c r="B94" t="s">
-        <v>10</v>
       </c>
       <c r="C94" t="s">
         <v>316</v>
@@ -3762,19 +3882,19 @@
         <v>330</v>
       </c>
       <c r="B99" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" t="s">
         <v>331</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F99" t="s">
         <v>332</v>
-      </c>
-      <c r="D99" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F99" t="s">
-        <v>333</v>
       </c>
       <c r="G99" t="s">
         <v>10</v>
@@ -3782,10 +3902,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
+        <v>333</v>
+      </c>
+      <c r="B100" t="s">
         <v>334</v>
-      </c>
-      <c r="B100" t="s">
-        <v>10</v>
       </c>
       <c r="C100" t="s">
         <v>335</v>
@@ -3808,19 +3928,19 @@
         <v>337</v>
       </c>
       <c r="B101" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" t="s">
         <v>338</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
+        <v>10</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F101" t="s">
         <v>339</v>
-      </c>
-      <c r="D101" t="s">
-        <v>10</v>
-      </c>
-      <c r="E101" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F101" t="s">
-        <v>340</v>
       </c>
       <c r="G101" t="s">
         <v>10</v>
@@ -3828,10 +3948,10 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
+        <v>340</v>
+      </c>
+      <c r="B102" t="s">
         <v>341</v>
-      </c>
-      <c r="B102" t="s">
-        <v>10</v>
       </c>
       <c r="C102" t="s">
         <v>342</v>
@@ -3854,19 +3974,19 @@
         <v>344</v>
       </c>
       <c r="B103" t="s">
+        <v>10</v>
+      </c>
+      <c r="C103" t="s">
         <v>345</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
+        <v>10</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F103" t="s">
         <v>346</v>
-      </c>
-      <c r="D103" t="s">
-        <v>10</v>
-      </c>
-      <c r="E103" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F103" t="s">
-        <v>347</v>
       </c>
       <c r="G103" t="s">
         <v>10</v>
@@ -3874,22 +3994,22 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
+        <v>347</v>
+      </c>
+      <c r="B104" t="s">
         <v>348</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>349</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
+        <v>10</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F104" t="s">
         <v>350</v>
-      </c>
-      <c r="D104" t="s">
-        <v>10</v>
-      </c>
-      <c r="E104" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F104" t="s">
-        <v>351</v>
       </c>
       <c r="G104" t="s">
         <v>10</v>
@@ -3897,22 +4017,22 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
+        <v>351</v>
+      </c>
+      <c r="B105" t="s">
         <v>352</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>353</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
+        <v>10</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F105" t="s">
         <v>354</v>
-      </c>
-      <c r="D105" t="s">
-        <v>10</v>
-      </c>
-      <c r="E105" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F105" t="s">
-        <v>355</v>
       </c>
       <c r="G105" t="s">
         <v>10</v>
@@ -3920,22 +4040,22 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
+        <v>355</v>
+      </c>
+      <c r="B106" t="s">
         <v>356</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>357</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
+        <v>10</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F106" t="s">
         <v>358</v>
-      </c>
-      <c r="D106" t="s">
-        <v>10</v>
-      </c>
-      <c r="E106" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F106" t="s">
-        <v>359</v>
       </c>
       <c r="G106" t="s">
         <v>10</v>
@@ -3943,22 +4063,22 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
+        <v>359</v>
+      </c>
+      <c r="B107" t="s">
         <v>360</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>361</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F107" t="s">
         <v>362</v>
-      </c>
-      <c r="D107" t="s">
-        <v>10</v>
-      </c>
-      <c r="E107" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F107" t="s">
-        <v>363</v>
       </c>
       <c r="G107" t="s">
         <v>10</v>
@@ -3966,22 +4086,22 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
+        <v>363</v>
+      </c>
+      <c r="B108" t="s">
         <v>364</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>365</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
+        <v>10</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F108" t="s">
         <v>366</v>
-      </c>
-      <c r="D108" t="s">
-        <v>10</v>
-      </c>
-      <c r="E108" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F108" t="s">
-        <v>367</v>
       </c>
       <c r="G108" t="s">
         <v>10</v>
@@ -3989,10 +4109,10 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
+        <v>367</v>
+      </c>
+      <c r="B109" t="s">
         <v>368</v>
-      </c>
-      <c r="B109" t="s">
-        <v>10</v>
       </c>
       <c r="C109" t="s">
         <v>369</v>
@@ -4038,19 +4158,19 @@
         <v>374</v>
       </c>
       <c r="B111" t="s">
+        <v>10</v>
+      </c>
+      <c r="C111" t="s">
         <v>375</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
+        <v>10</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F111" t="s">
         <v>376</v>
-      </c>
-      <c r="D111" t="s">
-        <v>10</v>
-      </c>
-      <c r="E111" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F111" t="s">
-        <v>377</v>
       </c>
       <c r="G111" t="s">
         <v>10</v>
@@ -4058,13 +4178,13 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
+        <v>377</v>
+      </c>
+      <c r="B112" t="s">
         <v>378</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
         <v>379</v>
-      </c>
-      <c r="C112" t="s">
-        <v>10</v>
       </c>
       <c r="D112" t="s">
         <v>10</v>
@@ -4084,10 +4204,10 @@
         <v>381</v>
       </c>
       <c r="B113" t="s">
-        <v>10</v>
+        <v>382</v>
       </c>
       <c r="C113" t="s">
-        <v>382</v>
+        <v>10</v>
       </c>
       <c r="D113" t="s">
         <v>10</v>
@@ -4153,19 +4273,19 @@
         <v>390</v>
       </c>
       <c r="B116" t="s">
+        <v>10</v>
+      </c>
+      <c r="C116" t="s">
         <v>391</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F116" t="s">
         <v>392</v>
-      </c>
-      <c r="D116" t="s">
-        <v>10</v>
-      </c>
-      <c r="E116" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F116" t="s">
-        <v>393</v>
       </c>
       <c r="G116" t="s">
         <v>10</v>
@@ -4173,10 +4293,10 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
+        <v>393</v>
+      </c>
+      <c r="B117" t="s">
         <v>394</v>
-      </c>
-      <c r="B117" t="s">
-        <v>10</v>
       </c>
       <c r="C117" t="s">
         <v>395</v>
@@ -4199,19 +4319,19 @@
         <v>397</v>
       </c>
       <c r="B118" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118" t="s">
         <v>398</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
+        <v>10</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F118" t="s">
         <v>399</v>
-      </c>
-      <c r="D118" t="s">
-        <v>10</v>
-      </c>
-      <c r="E118" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F118" t="s">
-        <v>400</v>
       </c>
       <c r="G118" t="s">
         <v>10</v>
@@ -4219,10 +4339,10 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
+        <v>400</v>
+      </c>
+      <c r="B119" t="s">
         <v>401</v>
-      </c>
-      <c r="B119" t="s">
-        <v>10</v>
       </c>
       <c r="C119" t="s">
         <v>402</v>
@@ -4337,10 +4457,10 @@
         <v>416</v>
       </c>
       <c r="B124" t="s">
+        <v>10</v>
+      </c>
+      <c r="C124" t="s">
         <v>417</v>
-      </c>
-      <c r="C124" t="s">
-        <v>10</v>
       </c>
       <c r="D124" t="s">
         <v>10</v>
@@ -4363,16 +4483,16 @@
         <v>420</v>
       </c>
       <c r="C125" t="s">
+        <v>10</v>
+      </c>
+      <c r="D125" t="s">
+        <v>10</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F125" t="s">
         <v>421</v>
-      </c>
-      <c r="D125" t="s">
-        <v>10</v>
-      </c>
-      <c r="E125" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F125" t="s">
-        <v>422</v>
       </c>
       <c r="G125" t="s">
         <v>10</v>
@@ -4380,10 +4500,10 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
+        <v>422</v>
+      </c>
+      <c r="B126" t="s">
         <v>423</v>
-      </c>
-      <c r="B126" t="s">
-        <v>10</v>
       </c>
       <c r="C126" t="s">
         <v>424</v>
@@ -4544,19 +4664,19 @@
         <v>444</v>
       </c>
       <c r="B133" t="s">
+        <v>10</v>
+      </c>
+      <c r="C133" t="s">
         <v>445</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="s">
+        <v>10</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F133" t="s">
         <v>446</v>
-      </c>
-      <c r="D133" t="s">
-        <v>10</v>
-      </c>
-      <c r="E133" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F133" t="s">
-        <v>447</v>
       </c>
       <c r="G133" t="s">
         <v>10</v>
@@ -4564,10 +4684,10 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
+        <v>447</v>
+      </c>
+      <c r="B134" t="s">
         <v>448</v>
-      </c>
-      <c r="B134" t="s">
-        <v>10</v>
       </c>
       <c r="C134" t="s">
         <v>449</v>
@@ -4582,6 +4702,236 @@
         <v>450</v>
       </c>
       <c r="G134" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>451</v>
+      </c>
+      <c r="B135" t="s">
+        <v>10</v>
+      </c>
+      <c r="C135" t="s">
+        <v>452</v>
+      </c>
+      <c r="D135" t="s">
+        <v>10</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F135" t="s">
+        <v>453</v>
+      </c>
+      <c r="G135" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>454</v>
+      </c>
+      <c r="B136" t="s">
+        <v>10</v>
+      </c>
+      <c r="C136" t="s">
+        <v>455</v>
+      </c>
+      <c r="D136" t="s">
+        <v>10</v>
+      </c>
+      <c r="E136" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F136" t="s">
+        <v>456</v>
+      </c>
+      <c r="G136" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>457</v>
+      </c>
+      <c r="B137" t="s">
+        <v>458</v>
+      </c>
+      <c r="C137" t="s">
+        <v>10</v>
+      </c>
+      <c r="D137" t="s">
+        <v>10</v>
+      </c>
+      <c r="E137" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F137" t="s">
+        <v>459</v>
+      </c>
+      <c r="G137" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>460</v>
+      </c>
+      <c r="B138" t="s">
+        <v>10</v>
+      </c>
+      <c r="C138" t="s">
+        <v>461</v>
+      </c>
+      <c r="D138" t="s">
+        <v>10</v>
+      </c>
+      <c r="E138" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F138" t="s">
+        <v>462</v>
+      </c>
+      <c r="G138" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>463</v>
+      </c>
+      <c r="B139" t="s">
+        <v>464</v>
+      </c>
+      <c r="C139" t="s">
+        <v>465</v>
+      </c>
+      <c r="D139" t="s">
+        <v>10</v>
+      </c>
+      <c r="E139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F139" t="s">
+        <v>466</v>
+      </c>
+      <c r="G139" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>467</v>
+      </c>
+      <c r="B140" t="s">
+        <v>468</v>
+      </c>
+      <c r="C140" t="s">
+        <v>10</v>
+      </c>
+      <c r="D140" t="s">
+        <v>10</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F140" t="s">
+        <v>469</v>
+      </c>
+      <c r="G140" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>470</v>
+      </c>
+      <c r="B141" t="s">
+        <v>471</v>
+      </c>
+      <c r="C141" t="s">
+        <v>10</v>
+      </c>
+      <c r="D141" t="s">
+        <v>10</v>
+      </c>
+      <c r="E141" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F141" t="s">
+        <v>472</v>
+      </c>
+      <c r="G141" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>473</v>
+      </c>
+      <c r="B142" t="s">
+        <v>474</v>
+      </c>
+      <c r="C142" t="s">
+        <v>475</v>
+      </c>
+      <c r="D142" t="s">
+        <v>10</v>
+      </c>
+      <c r="E142" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F142" t="s">
+        <v>476</v>
+      </c>
+      <c r="G142" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>477</v>
+      </c>
+      <c r="B143" t="s">
+        <v>478</v>
+      </c>
+      <c r="C143" t="s">
+        <v>479</v>
+      </c>
+      <c r="D143" t="s">
+        <v>10</v>
+      </c>
+      <c r="E143" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F143" t="s">
+        <v>480</v>
+      </c>
+      <c r="G143" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>481</v>
+      </c>
+      <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" t="s">
+        <v>482</v>
+      </c>
+      <c r="D144" t="s">
+        <v>10</v>
+      </c>
+      <c r="E144" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F144" t="s">
+        <v>483</v>
+      </c>
+      <c r="G144" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4592,7 +4942,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4600,7 +4950,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>451</v>
+        <v>484</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -4608,7 +4958,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>452</v>
+        <v>485</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -4616,7 +4966,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>453</v>
+        <v>486</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4624,7 +4974,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>454</v>
+        <v>487</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -4632,7 +4982,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>455</v>
+        <v>488</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -4640,7 +4990,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>456</v>
+        <v>489</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -4648,7 +4998,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>457</v>
+        <v>490</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -4656,7 +5006,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>458</v>
+        <v>491</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -4664,7 +5014,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>459</v>
+        <v>492</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -4672,7 +5022,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>460</v>
+        <v>493</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -4680,7 +5030,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>461</v>
+        <v>494</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -4688,7 +5038,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>462</v>
+        <v>495</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -4696,7 +5046,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>463</v>
+        <v>496</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -4704,7 +5054,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>464</v>
+        <v>497</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -4712,7 +5062,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>465</v>
+        <v>498</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -4720,7 +5070,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>466</v>
+        <v>499</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -4728,7 +5078,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>467</v>
+        <v>500</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -4736,7 +5086,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>468</v>
+        <v>501</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -4744,7 +5094,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>469</v>
+        <v>502</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -4752,7 +5102,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -4760,7 +5110,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>471</v>
+        <v>504</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -4768,7 +5118,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>472</v>
+        <v>505</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -4776,7 +5126,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>473</v>
+        <v>506</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -4784,7 +5134,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>474</v>
+        <v>507</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -4792,33 +5142,89 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>475</v>
+        <v>508</v>
       </c>
       <c r="B25" t="s">
-        <v>476</v>
+        <v>509</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>477</v>
+        <v>510</v>
       </c>
       <c r="B26" t="s">
-        <v>476</v>
+        <v>509</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>478</v>
+        <v>511</v>
       </c>
       <c r="B27" t="s">
-        <v>476</v>
+        <v>509</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>479</v>
+        <v>512</v>
       </c>
       <c r="B28" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>513</v>
+      </c>
+      <c r="B29" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>514</v>
+      </c>
+      <c r="B30" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>515</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>516</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>517</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>518</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>519</v>
+      </c>
+      <c r="B35" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: track the count of new notes and vocabulary entries added during the whole session
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="554">
   <si>
     <t>Word</t>
   </si>
@@ -1467,6 +1467,99 @@
     <t>2021-11-20 15:12:28.779915</t>
   </si>
   <si>
+    <t>congested</t>
+  </si>
+  <si>
+    <t>crowded</t>
+  </si>
+  <si>
+    <t>2021-11-20 22:32:31.286541</t>
+  </si>
+  <si>
+    <t>swerve</t>
+  </si>
+  <si>
+    <t>change or cause to change direction abruptly</t>
+  </si>
+  <si>
+    <t>veer</t>
+  </si>
+  <si>
+    <t>2021-11-20 22:33:54.608594</t>
+  </si>
+  <si>
+    <t>magnum opus</t>
+  </si>
+  <si>
+    <t>a work of art, music, or literature that is regarded as the most important or best work that an artist, composer, or writer has produced</t>
+  </si>
+  <si>
+    <t>2021-11-20 22:36:19.119537</t>
+  </si>
+  <si>
+    <t>anticipate</t>
+  </si>
+  <si>
+    <t>expect;predict</t>
+  </si>
+  <si>
+    <t>2021-11-20 22:36:48.436207</t>
+  </si>
+  <si>
+    <t>windfall</t>
+  </si>
+  <si>
+    <t>a large amount of money that is won or received unexpectedly</t>
+  </si>
+  <si>
+    <t>2021-11-20 22:52:03.527958</t>
+  </si>
+  <si>
+    <t>cushion</t>
+  </si>
+  <si>
+    <t>pillow;protection</t>
+  </si>
+  <si>
+    <t>2021-11-20 22:53:43.81857</t>
+  </si>
+  <si>
+    <t>diligently</t>
+  </si>
+  <si>
+    <t>in a way that shows care in one's work or duties</t>
+  </si>
+  <si>
+    <t>2021-11-20 22:55:00.4924</t>
+  </si>
+  <si>
+    <t>resilience</t>
+  </si>
+  <si>
+    <t>flexibility</t>
+  </si>
+  <si>
+    <t>2021-11-20 22:56:23.511821</t>
+  </si>
+  <si>
+    <t>parable</t>
+  </si>
+  <si>
+    <t>allegory</t>
+  </si>
+  <si>
+    <t>2021-11-20 22:57:34.943717</t>
+  </si>
+  <si>
+    <t>arbitrary</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>2021-11-20 22:59:11.038374</t>
+  </si>
+  <si>
     <t>content</t>
   </si>
   <si>
@@ -1573,6 +1666,15 @@
   </si>
   <si>
     <t>If you don't set boundaries - there won't be any</t>
+  </si>
+  <si>
+    <t>Give me 6 hours to chop down a tree and I will spend the first 4 sharpening the axe</t>
+  </si>
+  <si>
+    <t>The only thing we can expect (with any great certainty) is the unexpected</t>
+  </si>
+  <si>
+    <t>To attain knowledge add things every day. To attain wisdom subtract things every day</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1719,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G144"/>
+  <dimension ref="A1:G154"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -4935,6 +5037,236 @@
         <v>10</v>
       </c>
     </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>484</v>
+      </c>
+      <c r="B145" t="s">
+        <v>10</v>
+      </c>
+      <c r="C145" t="s">
+        <v>485</v>
+      </c>
+      <c r="D145" t="s">
+        <v>10</v>
+      </c>
+      <c r="E145" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F145" t="s">
+        <v>486</v>
+      </c>
+      <c r="G145" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>487</v>
+      </c>
+      <c r="B146" t="s">
+        <v>488</v>
+      </c>
+      <c r="C146" t="s">
+        <v>489</v>
+      </c>
+      <c r="D146" t="s">
+        <v>10</v>
+      </c>
+      <c r="E146" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F146" t="s">
+        <v>490</v>
+      </c>
+      <c r="G146" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>491</v>
+      </c>
+      <c r="B147" t="s">
+        <v>492</v>
+      </c>
+      <c r="C147" t="s">
+        <v>10</v>
+      </c>
+      <c r="D147" t="s">
+        <v>10</v>
+      </c>
+      <c r="E147" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F147" t="s">
+        <v>493</v>
+      </c>
+      <c r="G147" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>494</v>
+      </c>
+      <c r="B148" t="s">
+        <v>10</v>
+      </c>
+      <c r="C148" t="s">
+        <v>495</v>
+      </c>
+      <c r="D148" t="s">
+        <v>10</v>
+      </c>
+      <c r="E148" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F148" t="s">
+        <v>496</v>
+      </c>
+      <c r="G148" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>497</v>
+      </c>
+      <c r="B149" t="s">
+        <v>498</v>
+      </c>
+      <c r="C149" t="s">
+        <v>10</v>
+      </c>
+      <c r="D149" t="s">
+        <v>10</v>
+      </c>
+      <c r="E149" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F149" t="s">
+        <v>499</v>
+      </c>
+      <c r="G149" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>500</v>
+      </c>
+      <c r="B150" t="s">
+        <v>10</v>
+      </c>
+      <c r="C150" t="s">
+        <v>501</v>
+      </c>
+      <c r="D150" t="s">
+        <v>10</v>
+      </c>
+      <c r="E150" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F150" t="s">
+        <v>502</v>
+      </c>
+      <c r="G150" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>503</v>
+      </c>
+      <c r="B151" t="s">
+        <v>504</v>
+      </c>
+      <c r="C151" t="s">
+        <v>10</v>
+      </c>
+      <c r="D151" t="s">
+        <v>10</v>
+      </c>
+      <c r="E151" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F151" t="s">
+        <v>505</v>
+      </c>
+      <c r="G151" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>506</v>
+      </c>
+      <c r="B152" t="s">
+        <v>10</v>
+      </c>
+      <c r="C152" t="s">
+        <v>507</v>
+      </c>
+      <c r="D152" t="s">
+        <v>10</v>
+      </c>
+      <c r="E152" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F152" t="s">
+        <v>508</v>
+      </c>
+      <c r="G152" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>509</v>
+      </c>
+      <c r="B153" t="s">
+        <v>10</v>
+      </c>
+      <c r="C153" t="s">
+        <v>510</v>
+      </c>
+      <c r="D153" t="s">
+        <v>10</v>
+      </c>
+      <c r="E153" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F153" t="s">
+        <v>511</v>
+      </c>
+      <c r="G153" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>512</v>
+      </c>
+      <c r="B154" t="s">
+        <v>10</v>
+      </c>
+      <c r="C154" t="s">
+        <v>513</v>
+      </c>
+      <c r="D154" t="s">
+        <v>10</v>
+      </c>
+      <c r="E154" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F154" t="s">
+        <v>514</v>
+      </c>
+      <c r="G154" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -4942,7 +5274,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4950,7 +5282,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>484</v>
+        <v>515</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -4958,7 +5290,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -4966,7 +5298,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>486</v>
+        <v>517</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4974,7 +5306,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>487</v>
+        <v>518</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -4982,7 +5314,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>488</v>
+        <v>519</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -4990,7 +5322,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>489</v>
+        <v>520</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -4998,7 +5330,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>490</v>
+        <v>521</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -5006,7 +5338,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>491</v>
+        <v>522</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -5014,7 +5346,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>492</v>
+        <v>523</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -5022,7 +5354,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>493</v>
+        <v>524</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -5030,7 +5362,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>494</v>
+        <v>525</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -5038,7 +5370,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>495</v>
+        <v>526</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -5046,7 +5378,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>496</v>
+        <v>527</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -5054,7 +5386,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>497</v>
+        <v>528</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -5062,7 +5394,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>498</v>
+        <v>529</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -5070,7 +5402,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>499</v>
+        <v>530</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -5078,7 +5410,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>500</v>
+        <v>531</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -5086,7 +5418,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>501</v>
+        <v>532</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -5094,7 +5426,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>502</v>
+        <v>533</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -5102,7 +5434,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>503</v>
+        <v>534</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -5110,7 +5442,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>504</v>
+        <v>535</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -5118,7 +5450,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>505</v>
+        <v>536</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -5126,7 +5458,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>506</v>
+        <v>537</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -5134,7 +5466,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>507</v>
+        <v>538</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -5142,55 +5474,55 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>508</v>
+        <v>539</v>
       </c>
       <c r="B25" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>510</v>
+        <v>541</v>
       </c>
       <c r="B26" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>511</v>
+        <v>542</v>
       </c>
       <c r="B27" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>512</v>
+        <v>543</v>
       </c>
       <c r="B28" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>513</v>
+        <v>544</v>
       </c>
       <c r="B29" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>514</v>
+        <v>545</v>
       </c>
       <c r="B30" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>515</v>
+        <v>546</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -5198,7 +5530,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>516</v>
+        <v>547</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -5206,7 +5538,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>517</v>
+        <v>548</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -5214,7 +5546,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>518</v>
+        <v>549</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -5222,9 +5554,33 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>519</v>
+        <v>550</v>
       </c>
       <c r="B35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>551</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>552</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>553</v>
+      </c>
+      <c r="B38" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: display note by id
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ENGLISH" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="625">
   <si>
     <t xml:space="preserve">Word</t>
   </si>
@@ -1664,12 +1664,96 @@
     <t xml:space="preserve">2021-11-21 01:56:39.679729</t>
   </si>
   <si>
+    <t xml:space="preserve">opulent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">luxurious;wealthy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-21 15:33:36.099685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">characteristic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-21 15:35:43.609799</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tenet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">principle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-21 15:37:00.336208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tempt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-21 15:37:54.117744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proverb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-21 15:38:34.634497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insipid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tasteless;weak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-21 15:40:27.314993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">startling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remarkable;surprising;astonishing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-21 15:41:25.484576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plateau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a state of little or no change following a period of activity or progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-21 15:42:35.633005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">counterfeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-21 15:44:40.04142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repercussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11-21 15:45:55.726065</t>
+  </si>
+  <si>
     <t xml:space="preserve">content</t>
   </si>
   <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
     <t xml:space="preserve">Without great solitude no serious work is possible</t>
   </si>
   <si>
@@ -1809,6 +1893,9 @@
   </si>
   <si>
     <t xml:space="preserve">Get the future out of your head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarity equals success</t>
   </si>
 </sst>
 </file>
@@ -1904,10 +1991,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G164"/>
+  <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A136" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H167" activeCellId="0" sqref="H167"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A142" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H165" activeCellId="0" sqref="H165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4224,7 +4311,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>514</v>
       </c>
@@ -4238,7 +4325,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
         <v>517</v>
       </c>
@@ -4255,7 +4342,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>521</v>
       </c>
@@ -4269,7 +4356,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>524</v>
       </c>
@@ -4286,7 +4373,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>528</v>
       </c>
@@ -4300,7 +4387,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
         <v>531</v>
       </c>
@@ -4317,7 +4404,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
         <v>535</v>
       </c>
@@ -4331,7 +4418,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>538</v>
       </c>
@@ -4345,7 +4432,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
         <v>541</v>
       </c>
@@ -4359,7 +4446,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
         <v>544</v>
       </c>
@@ -4371,6 +4458,147 @@
       </c>
       <c r="F164" s="0" t="s">
         <v>546</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="C166" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="E166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F166" s="0" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="C167" s="0" t="s">
+        <v>551</v>
+      </c>
+      <c r="E167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F167" s="0" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="C168" s="0" t="s">
+        <v>554</v>
+      </c>
+      <c r="E168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F168" s="0" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>556</v>
+      </c>
+      <c r="C169" s="0" t="s">
+        <v>557</v>
+      </c>
+      <c r="E169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F169" s="0" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>559</v>
+      </c>
+      <c r="C170" s="0" t="s">
+        <v>560</v>
+      </c>
+      <c r="E170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F170" s="0" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="C171" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="E171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F171" s="0" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>565</v>
+      </c>
+      <c r="C172" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="E172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F172" s="0" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="E173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F173" s="0" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="C174" s="0" t="s">
+        <v>572</v>
+      </c>
+      <c r="E174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F174" s="0" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>574</v>
+      </c>
+      <c r="C175" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F175" s="0" t="s">
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -4391,15 +4619,15 @@
   </sheetPr>
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K29" activeCellId="0" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>547</v>
+        <v>576</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>6</v>
@@ -4407,264 +4635,264 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>548</v>
+        <v>577</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>549</v>
+        <v>578</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>550</v>
+        <v>579</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>551</v>
+        <v>580</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>552</v>
+        <v>581</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>553</v>
+        <v>582</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>554</v>
+        <v>583</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>555</v>
+        <v>584</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>556</v>
+        <v>585</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>557</v>
+        <v>586</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>558</v>
+        <v>587</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>559</v>
+        <v>588</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>560</v>
+        <v>589</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>561</v>
+        <v>590</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>562</v>
+        <v>591</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>563</v>
+        <v>592</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>564</v>
+        <v>593</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>565</v>
+        <v>594</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>566</v>
+        <v>595</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>567</v>
+        <v>596</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>568</v>
+        <v>597</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>569</v>
+        <v>598</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>570</v>
+        <v>599</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>571</v>
+        <v>600</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>572</v>
+        <v>602</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>573</v>
+        <v>601</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>574</v>
+        <v>603</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>573</v>
+        <v>601</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>575</v>
+        <v>604</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>573</v>
+        <v>601</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>576</v>
+        <v>605</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>573</v>
+        <v>601</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>577</v>
+        <v>606</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>573</v>
+        <v>601</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>578</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>573</v>
+        <v>607</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>579</v>
+        <v>608</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>580</v>
+        <v>609</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>581</v>
+        <v>610</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>582</v>
+        <v>611</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>583</v>
+        <v>612</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>584</v>
+        <v>613</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>585</v>
+        <v>614</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>586</v>
+        <v>615</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>587</v>
+        <v>616</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>588</v>
+        <v>617</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>589</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>573</v>
+        <v>618</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>590</v>
+        <v>619</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>591</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>573</v>
+        <v>620</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>592</v>
+        <v>621</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>593</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>573</v>
+        <v>622</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>594</v>
+        <v>623</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>595</v>
+        <v>624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: delete vocabulary entry by id
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="673">
   <si>
     <t>Word</t>
   </si>
@@ -1818,6 +1818,51 @@
     <t>2021-11-22 12:41:23.881295</t>
   </si>
   <si>
+    <t>astounding</t>
+  </si>
+  <si>
+    <t>amazing;impressive;notable</t>
+  </si>
+  <si>
+    <t>2021-11-23 13:31:52.160918</t>
+  </si>
+  <si>
+    <t>tangible</t>
+  </si>
+  <si>
+    <t>real;touchable</t>
+  </si>
+  <si>
+    <t>2021-11-23 13:32:51.714678</t>
+  </si>
+  <si>
+    <t>growl</t>
+  </si>
+  <si>
+    <t>snarl;say roughly</t>
+  </si>
+  <si>
+    <t>2021-11-23 13:38:21.392315</t>
+  </si>
+  <si>
+    <t>impose</t>
+  </si>
+  <si>
+    <t>force (an unwelcome decision or ruling) on someone</t>
+  </si>
+  <si>
+    <t>2021-11-23 13:40:32.909102</t>
+  </si>
+  <si>
+    <t>revolt</t>
+  </si>
+  <si>
+    <t>rebel</t>
+  </si>
+  <si>
+    <t>2021-11-23 13:41:24.307841</t>
+  </si>
+  <si>
     <t>content</t>
   </si>
   <si>
@@ -1963,6 +2008,30 @@
   </si>
   <si>
     <t>Clarity equals success</t>
+  </si>
+  <si>
+    <t>Same habits, same results</t>
+  </si>
+  <si>
+    <t>habit</t>
+  </si>
+  <si>
+    <t>Changes that seem small and unimportant at first will compound into remarkable results if you are willing to stick with them for years</t>
+  </si>
+  <si>
+    <t>In the long run, the quality of our lives often depends on the quality of our habits</t>
+  </si>
+  <si>
+    <t>Mastery requires patience</t>
+  </si>
+  <si>
+    <t>Goals are good for setting a direction, but systems are best for making progress</t>
+  </si>
+  <si>
+    <t>True behavior change is identity change</t>
+  </si>
+  <si>
+    <t>Habits create freedom</t>
   </si>
 </sst>
 </file>
@@ -2007,7 +2076,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H181"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -6719,6 +6788,136 @@
         <v>11</v>
       </c>
     </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>601</v>
+      </c>
+      <c r="B182" t="s">
+        <v>11</v>
+      </c>
+      <c r="C182" t="s">
+        <v>602</v>
+      </c>
+      <c r="D182" t="s">
+        <v>11</v>
+      </c>
+      <c r="E182" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F182" t="s">
+        <v>603</v>
+      </c>
+      <c r="G182" t="s">
+        <v>11</v>
+      </c>
+      <c r="H182" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>604</v>
+      </c>
+      <c r="B183" t="s">
+        <v>11</v>
+      </c>
+      <c r="C183" t="s">
+        <v>605</v>
+      </c>
+      <c r="D183" t="s">
+        <v>11</v>
+      </c>
+      <c r="E183" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F183" t="s">
+        <v>606</v>
+      </c>
+      <c r="G183" t="s">
+        <v>11</v>
+      </c>
+      <c r="H183" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>607</v>
+      </c>
+      <c r="B184" t="s">
+        <v>11</v>
+      </c>
+      <c r="C184" t="s">
+        <v>608</v>
+      </c>
+      <c r="D184" t="s">
+        <v>11</v>
+      </c>
+      <c r="E184" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F184" t="s">
+        <v>609</v>
+      </c>
+      <c r="G184" t="s">
+        <v>11</v>
+      </c>
+      <c r="H184" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>610</v>
+      </c>
+      <c r="B185" t="s">
+        <v>611</v>
+      </c>
+      <c r="C185" t="s">
+        <v>11</v>
+      </c>
+      <c r="D185" t="s">
+        <v>11</v>
+      </c>
+      <c r="E185" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F185" t="s">
+        <v>612</v>
+      </c>
+      <c r="G185" t="s">
+        <v>11</v>
+      </c>
+      <c r="H185" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>613</v>
+      </c>
+      <c r="B186" t="s">
+        <v>11</v>
+      </c>
+      <c r="C186" t="s">
+        <v>614</v>
+      </c>
+      <c r="D186" t="s">
+        <v>11</v>
+      </c>
+      <c r="E186" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F186" t="s">
+        <v>615</v>
+      </c>
+      <c r="G186" t="s">
+        <v>11</v>
+      </c>
+      <c r="H186" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -6726,7 +6925,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6734,7 +6933,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>601</v>
+        <v>616</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -6742,7 +6941,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>602</v>
+        <v>617</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -6750,7 +6949,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>603</v>
+        <v>618</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -6758,7 +6957,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>604</v>
+        <v>619</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -6766,7 +6965,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>605</v>
+        <v>620</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -6774,7 +6973,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>606</v>
+        <v>621</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -6782,7 +6981,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>607</v>
+        <v>622</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -6790,7 +6989,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>608</v>
+        <v>623</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -6798,7 +6997,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>609</v>
+        <v>624</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -6806,7 +7005,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>610</v>
+        <v>625</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -6814,7 +7013,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>611</v>
+        <v>626</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -6822,7 +7021,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>612</v>
+        <v>627</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -6830,7 +7029,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>613</v>
+        <v>628</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -6838,7 +7037,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>614</v>
+        <v>629</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -6846,7 +7045,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>615</v>
+        <v>630</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -6854,7 +7053,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>616</v>
+        <v>631</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -6862,7 +7061,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>617</v>
+        <v>632</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -6870,7 +7069,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>618</v>
+        <v>633</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -6878,7 +7077,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>619</v>
+        <v>634</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
@@ -6886,7 +7085,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>620</v>
+        <v>635</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -6894,7 +7093,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>621</v>
+        <v>636</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -6902,7 +7101,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>622</v>
+        <v>637</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -6910,7 +7109,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>623</v>
+        <v>638</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
@@ -6918,7 +7117,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>624</v>
+        <v>639</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
@@ -6926,55 +7125,55 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>625</v>
+        <v>640</v>
       </c>
       <c r="B25" t="s">
-        <v>626</v>
+        <v>641</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>627</v>
+        <v>642</v>
       </c>
       <c r="B26" t="s">
-        <v>626</v>
+        <v>641</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>628</v>
+        <v>643</v>
       </c>
       <c r="B27" t="s">
-        <v>626</v>
+        <v>641</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>629</v>
+        <v>644</v>
       </c>
       <c r="B28" t="s">
-        <v>626</v>
+        <v>641</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>630</v>
+        <v>645</v>
       </c>
       <c r="B29" t="s">
-        <v>626</v>
+        <v>641</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>631</v>
+        <v>646</v>
       </c>
       <c r="B30" t="s">
-        <v>626</v>
+        <v>641</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>632</v>
+        <v>647</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -6982,7 +7181,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>633</v>
+        <v>648</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
@@ -6990,7 +7189,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>634</v>
+        <v>649</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
@@ -6998,7 +7197,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>635</v>
+        <v>650</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
@@ -7006,7 +7205,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>636</v>
+        <v>651</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
@@ -7014,7 +7213,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>637</v>
+        <v>652</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
@@ -7022,7 +7221,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>638</v>
+        <v>653</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
@@ -7030,7 +7229,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>639</v>
+        <v>654</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
@@ -7038,7 +7237,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>640</v>
+        <v>655</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
@@ -7046,7 +7245,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>641</v>
+        <v>656</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
@@ -7054,15 +7253,15 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>642</v>
+        <v>657</v>
       </c>
       <c r="B41" t="s">
-        <v>626</v>
+        <v>641</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>643</v>
+        <v>658</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
@@ -7070,15 +7269,15 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>644</v>
+        <v>659</v>
       </c>
       <c r="B43" t="s">
-        <v>626</v>
+        <v>641</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>645</v>
+        <v>660</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
@@ -7086,15 +7285,15 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>646</v>
+        <v>661</v>
       </c>
       <c r="B45" t="s">
-        <v>626</v>
+        <v>641</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>647</v>
+        <v>662</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -7102,7 +7301,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>648</v>
+        <v>663</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
@@ -7110,10 +7309,66 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>649</v>
+        <v>664</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>665</v>
+      </c>
+      <c r="B49" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>667</v>
+      </c>
+      <c r="B50" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>668</v>
+      </c>
+      <c r="B51" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>669</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>670</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>671</v>
+      </c>
+      <c r="B54" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>672</v>
+      </c>
+      <c r="B55" t="s">
+        <v>666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>